<commit_message>
modelo atualizado para deploy
</commit_message>
<xml_diff>
--- a/input/8.xlsx
+++ b/input/8.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
   <si>
     <t>Data/Hora*</t>
   </si>
@@ -33,6 +33,9 @@
   </si>
   <si>
     <t>Vazão (m3/s)</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -435,3866 +438,3866 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1">
-        <v>45954</v>
+        <v>45960</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D3">
-        <v>1.76</v>
+        <v>2.12</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="G3">
-        <v>1.47</v>
+        <v>1.87</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1">
-        <v>45954.041666667</v>
+        <v>45960.041666667</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="C4">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D4">
-        <v>1.76</v>
+        <v>2.12</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="G4">
-        <v>1.47</v>
+        <v>1.87</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1">
-        <v>45954.083333333</v>
+        <v>45960.083333333</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D5">
-        <v>1.85</v>
+        <v>2.12</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="G5">
-        <v>1.47</v>
+        <v>1.87</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1">
-        <v>45954.125</v>
+        <v>45960.125</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
       <c r="C6">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D6">
-        <v>1.76</v>
+        <v>2.12</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="G6">
-        <v>1.47</v>
+        <v>1.73</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1">
-        <v>45954.166666667</v>
+        <v>45960.166666667</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C7">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D7">
-        <v>1.76</v>
+        <v>2.12</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="G7">
-        <v>1.47</v>
+        <v>1.73</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1">
-        <v>45954.208333333</v>
+        <v>45960.208333333</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
       <c r="C8">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D8">
-        <v>1.76</v>
+        <v>2.12</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="G8">
-        <v>1.34</v>
+        <v>1.73</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1">
-        <v>45954.25</v>
+        <v>45960.25</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="C9">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D9">
-        <v>1.76</v>
+        <v>2.12</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="G9">
-        <v>1.34</v>
+        <v>1.87</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1">
-        <v>45954.291666667</v>
+        <v>45960.291666667</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C10">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="D10">
-        <v>1.76</v>
+        <v>2.21</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="G10">
-        <v>1.34</v>
+        <v>1.73</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1">
-        <v>45954.333333333</v>
+        <v>45960.333333333</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
       <c r="C11">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="D11">
-        <v>1.76</v>
+        <v>2.4</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="G11">
-        <v>1.34</v>
+        <v>1.73</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1">
-        <v>45954.375</v>
+        <v>45960.375</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
       <c r="C12">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="D12">
-        <v>1.68</v>
+        <v>2.3</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="G12">
-        <v>1.47</v>
+        <v>1.87</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1">
-        <v>45954.416666667</v>
+        <v>45960.416666667</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
       <c r="C13">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="D13">
-        <v>1.6</v>
+        <v>2.12</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="F13">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="G13">
-        <v>1.47</v>
+        <v>1.87</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="1">
-        <v>45954.458333333</v>
+        <v>45960.458333333</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
       <c r="C14">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="D14">
-        <v>1.6</v>
+        <v>2.12</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="G14">
-        <v>1.47</v>
+        <v>1.87</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="1">
-        <v>45954.5</v>
+        <v>45960.5</v>
       </c>
       <c r="B15">
         <v>0</v>
       </c>
       <c r="C15">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="D15">
-        <v>1.52</v>
+        <v>2.03</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
       <c r="F15">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="G15">
-        <v>1.47</v>
+        <v>1.87</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="1">
-        <v>45954.541666667</v>
+        <v>45960.541666667</v>
       </c>
       <c r="B16">
         <v>0</v>
       </c>
       <c r="C16">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="D16">
-        <v>1.6</v>
+        <v>2.03</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="F16">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="G16">
-        <v>1.47</v>
+        <v>1.87</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="1">
-        <v>45954.583333333</v>
+        <v>45960.583333333</v>
       </c>
       <c r="B17">
         <v>0</v>
       </c>
       <c r="C17">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="D17">
-        <v>1.6</v>
+        <v>2.03</v>
       </c>
       <c r="E17">
         <v>0</v>
       </c>
       <c r="F17">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="G17">
-        <v>1.47</v>
+        <v>1.87</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="1">
-        <v>45954.625</v>
+        <v>45960.625</v>
       </c>
       <c r="B18">
         <v>0</v>
       </c>
       <c r="C18">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="D18">
-        <v>1.6</v>
+        <v>2.03</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="F18">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="G18">
-        <v>1.47</v>
+        <v>1.73</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="1">
-        <v>45954.666666667</v>
+        <v>45960.666666667</v>
       </c>
       <c r="B19">
         <v>0</v>
       </c>
       <c r="C19">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="D19">
-        <v>1.6</v>
+        <v>2.03</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
       <c r="F19">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="G19">
-        <v>1.47</v>
+        <v>1.73</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="1">
-        <v>45954.708333333</v>
+        <v>45960.708333333</v>
       </c>
       <c r="B20">
         <v>0</v>
       </c>
       <c r="C20">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="D20">
-        <v>1.6</v>
+        <v>2.03</v>
       </c>
       <c r="E20">
         <v>0</v>
       </c>
       <c r="F20">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="G20">
-        <v>1.47</v>
+        <v>1.73</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="1">
-        <v>45954.75</v>
+        <v>45960.75</v>
       </c>
       <c r="B21">
         <v>0</v>
       </c>
       <c r="C21">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="D21">
-        <v>1.6</v>
+        <v>2.03</v>
       </c>
       <c r="E21">
         <v>0</v>
       </c>
       <c r="F21">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="G21">
-        <v>1.47</v>
+        <v>1.73</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="1">
-        <v>45954.791666667</v>
+        <v>45960.791666667</v>
       </c>
       <c r="B22">
         <v>0</v>
       </c>
       <c r="C22">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="D22">
-        <v>1.6</v>
+        <v>2.03</v>
       </c>
       <c r="E22">
         <v>0</v>
       </c>
       <c r="F22">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="G22">
-        <v>1.47</v>
+        <v>1.73</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="1">
-        <v>45954.833333333</v>
+        <v>45960.833333333</v>
       </c>
       <c r="B23">
         <v>0</v>
       </c>
       <c r="C23">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="D23">
-        <v>1.6</v>
+        <v>2.03</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
       <c r="F23">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="G23">
-        <v>1.47</v>
+        <v>1.73</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="1">
-        <v>45954.875</v>
+        <v>45960.875</v>
       </c>
       <c r="B24">
         <v>0</v>
       </c>
       <c r="C24">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D24">
-        <v>1.68</v>
+        <v>2.03</v>
       </c>
       <c r="E24">
         <v>0</v>
       </c>
       <c r="F24">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="G24">
-        <v>1.34</v>
+        <v>1.73</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="1">
-        <v>45954.916666667</v>
+        <v>45960.916666667</v>
       </c>
       <c r="B25">
         <v>0</v>
       </c>
       <c r="C25">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="D25">
-        <v>1.6</v>
+        <v>2.03</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
       <c r="F25">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="G25">
-        <v>1.34</v>
+        <v>1.73</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="1">
-        <v>45954.958333333</v>
+        <v>45960.958333333</v>
       </c>
       <c r="B26">
         <v>0</v>
       </c>
       <c r="C26">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="D26">
-        <v>1.6</v>
+        <v>1.94</v>
       </c>
       <c r="E26">
         <v>0</v>
       </c>
       <c r="F26">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="G26">
-        <v>1.34</v>
+        <v>1.59</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="1">
-        <v>45955</v>
+        <v>45961</v>
       </c>
       <c r="B27">
         <v>0</v>
       </c>
       <c r="C27">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="D27">
-        <v>1.6</v>
+        <v>1.94</v>
       </c>
       <c r="E27">
         <v>0</v>
       </c>
       <c r="F27">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="G27">
-        <v>1.34</v>
+        <v>1.73</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="1">
-        <v>45955.041666667</v>
+        <v>45961.041666667</v>
       </c>
       <c r="B28">
         <v>0</v>
       </c>
       <c r="C28">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="D28">
-        <v>1.6</v>
+        <v>1.94</v>
       </c>
       <c r="E28">
         <v>0</v>
       </c>
       <c r="F28">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="G28">
-        <v>1.34</v>
+        <v>1.59</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="1">
-        <v>45955.083333333</v>
+        <v>45961.083333333</v>
       </c>
       <c r="B29">
         <v>0</v>
       </c>
       <c r="C29">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="D29">
-        <v>1.6</v>
+        <v>1.94</v>
       </c>
       <c r="E29">
         <v>0</v>
       </c>
       <c r="F29">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="G29">
-        <v>1.23</v>
+        <v>1.59</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="1">
-        <v>45955.125</v>
+        <v>45961.125</v>
       </c>
       <c r="B30">
         <v>0</v>
       </c>
       <c r="C30">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="D30">
-        <v>1.6</v>
+        <v>2.03</v>
       </c>
       <c r="E30">
         <v>0</v>
       </c>
       <c r="F30">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="G30">
-        <v>1.23</v>
+        <v>1.59</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="1">
-        <v>45955.166666667</v>
+        <v>45961.166666667</v>
       </c>
       <c r="B31">
         <v>0</v>
       </c>
       <c r="C31">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="D31">
-        <v>1.6</v>
+        <v>1.94</v>
       </c>
       <c r="E31">
         <v>0</v>
       </c>
       <c r="F31">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="G31">
-        <v>1.23</v>
+        <v>1.59</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="1">
-        <v>45955.208333333</v>
+        <v>45961.208333333</v>
       </c>
       <c r="B32">
         <v>0</v>
       </c>
       <c r="C32">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="D32">
-        <v>1.6</v>
+        <v>1.94</v>
       </c>
       <c r="E32">
         <v>0</v>
       </c>
       <c r="F32">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="G32">
-        <v>1.23</v>
+        <v>1.59</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="1">
-        <v>45955.25</v>
+        <v>45961.25</v>
       </c>
       <c r="B33">
         <v>0</v>
       </c>
       <c r="C33">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="D33">
-        <v>1.6</v>
+        <v>1.94</v>
       </c>
       <c r="E33">
         <v>0</v>
       </c>
       <c r="F33">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="G33">
-        <v>1.23</v>
+        <v>1.47</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="1">
-        <v>45955.291666667</v>
+        <v>45961.291666667</v>
       </c>
       <c r="B34">
         <v>0</v>
       </c>
       <c r="C34">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D34">
-        <v>1.52</v>
+        <v>1.94</v>
       </c>
       <c r="E34">
         <v>0</v>
       </c>
       <c r="F34">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="G34">
-        <v>1.23</v>
+        <v>1.47</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="1">
-        <v>45955.333333333</v>
+        <v>45961.333333333</v>
       </c>
       <c r="B35">
         <v>0</v>
       </c>
       <c r="C35">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D35">
-        <v>1.52</v>
+        <v>1.94</v>
       </c>
       <c r="E35">
         <v>0</v>
       </c>
       <c r="F35">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="G35">
-        <v>1.34</v>
+        <v>1.59</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="1">
-        <v>45955.375</v>
+        <v>45961.375</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C36">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D36">
-        <v>1.52</v>
+        <v>1.94</v>
       </c>
       <c r="E36">
         <v>0</v>
       </c>
       <c r="F36">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="G36">
-        <v>1.34</v>
+        <v>1.59</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="1">
-        <v>45955.416666667</v>
+        <v>45961.416666667</v>
       </c>
       <c r="B37">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="C37">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D37">
-        <v>1.52</v>
+        <v>1.94</v>
       </c>
       <c r="E37">
         <v>0</v>
       </c>
       <c r="F37">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="G37">
-        <v>1.34</v>
+        <v>1.73</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="1">
-        <v>45955.458333333</v>
+        <v>45961.458333333</v>
       </c>
       <c r="B38">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C38">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="D38">
-        <v>1.44</v>
+        <v>2.91</v>
       </c>
       <c r="E38">
         <v>0</v>
       </c>
       <c r="F38">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="G38">
-        <v>1.34</v>
+        <v>2.17</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="1">
-        <v>45955.5</v>
+        <v>45961.5</v>
       </c>
       <c r="B39">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="C39">
-        <v>97</v>
+        <v>130</v>
       </c>
       <c r="D39">
-        <v>1.44</v>
+        <v>4.99</v>
       </c>
       <c r="E39">
         <v>0</v>
       </c>
       <c r="F39">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="G39">
-        <v>1.34</v>
+        <v>2.17</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="1">
-        <v>45955.541666667</v>
+        <v>45961.541666667</v>
       </c>
       <c r="B40">
         <v>0</v>
       </c>
       <c r="C40">
-        <v>97</v>
+        <v>125</v>
       </c>
       <c r="D40">
-        <v>1.44</v>
-      </c>
-      <c r="E40">
-        <v>0</v>
-      </c>
-      <c r="F40">
-        <v>146</v>
-      </c>
-      <c r="G40">
-        <v>1.34</v>
+        <v>4.33</v>
+      </c>
+      <c r="E40" t="s">
+        <v>6</v>
+      </c>
+      <c r="F40" t="s">
+        <v>6</v>
+      </c>
+      <c r="G40" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="1">
-        <v>45955.583333333</v>
+        <v>45961.583333333</v>
       </c>
       <c r="B41">
         <v>0</v>
       </c>
       <c r="C41">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="D41">
-        <v>1.44</v>
+        <v>3.24</v>
       </c>
       <c r="E41">
         <v>0</v>
       </c>
       <c r="F41">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="G41">
-        <v>1.47</v>
+        <v>2.17</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="1">
-        <v>45955.625</v>
+        <v>45961.625</v>
       </c>
       <c r="B42">
         <v>0</v>
       </c>
       <c r="C42">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="D42">
-        <v>1.44</v>
+        <v>2.7</v>
       </c>
       <c r="E42">
         <v>0</v>
       </c>
       <c r="F42">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="G42">
-        <v>1.47</v>
+        <v>2.01</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="1">
-        <v>45955.666666667</v>
+        <v>45961.666666667</v>
       </c>
       <c r="B43">
         <v>0</v>
       </c>
       <c r="C43">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="D43">
-        <v>1.44</v>
+        <v>2.5</v>
       </c>
       <c r="E43">
         <v>0</v>
       </c>
       <c r="F43">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="G43">
-        <v>1.47</v>
+        <v>2.01</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="1">
-        <v>45955.708333333</v>
+        <v>45961.708333333</v>
       </c>
       <c r="B44">
         <v>0</v>
       </c>
       <c r="C44">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="D44">
-        <v>1.44</v>
+        <v>2.3</v>
       </c>
       <c r="E44">
         <v>0</v>
       </c>
       <c r="F44">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="G44">
-        <v>1.34</v>
+        <v>1.87</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="1">
-        <v>45955.75</v>
+        <v>45961.75</v>
       </c>
       <c r="B45">
         <v>0</v>
       </c>
       <c r="C45">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="D45">
-        <v>1.44</v>
+        <v>2.3</v>
       </c>
       <c r="E45">
         <v>0</v>
       </c>
       <c r="F45">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="G45">
-        <v>1.34</v>
+        <v>1.87</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="1">
-        <v>45955.791666667</v>
+        <v>45961.791666667</v>
       </c>
       <c r="B46">
         <v>0</v>
       </c>
       <c r="C46">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="D46">
-        <v>1.44</v>
+        <v>2.21</v>
       </c>
       <c r="E46">
         <v>0</v>
       </c>
       <c r="F46">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="G46">
-        <v>1.34</v>
+        <v>1.73</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="1">
-        <v>45955.833333333</v>
+        <v>45961.833333333</v>
       </c>
       <c r="B47">
         <v>0</v>
       </c>
       <c r="C47">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="D47">
-        <v>1.44</v>
+        <v>2.21</v>
       </c>
       <c r="E47">
         <v>0</v>
       </c>
       <c r="F47">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="G47">
-        <v>1.34</v>
+        <v>1.73</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="1">
-        <v>45955.875</v>
+        <v>45961.875</v>
       </c>
       <c r="B48">
         <v>0</v>
       </c>
       <c r="C48">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="D48">
-        <v>1.52</v>
+        <v>2.21</v>
       </c>
       <c r="E48">
         <v>0</v>
       </c>
       <c r="F48">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="G48">
-        <v>1.34</v>
+        <v>1.73</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="1">
-        <v>45955.916666667</v>
+        <v>45961.916666667</v>
       </c>
       <c r="B49">
         <v>0</v>
       </c>
       <c r="C49">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="D49">
-        <v>1.44</v>
+        <v>2.21</v>
       </c>
       <c r="E49">
         <v>0</v>
       </c>
       <c r="F49">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="G49">
-        <v>1.34</v>
+        <v>1.73</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="1">
-        <v>45955.958333333</v>
+        <v>45961.958333333</v>
       </c>
       <c r="B50">
         <v>0</v>
       </c>
       <c r="C50">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="D50">
-        <v>1.44</v>
+        <v>2.12</v>
       </c>
       <c r="E50">
         <v>0</v>
       </c>
       <c r="F50">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="G50">
-        <v>1.34</v>
+        <v>1.87</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="1">
-        <v>45956</v>
+        <v>45962</v>
       </c>
       <c r="B51">
         <v>0</v>
       </c>
       <c r="C51">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="D51">
-        <v>1.44</v>
+        <v>2.21</v>
       </c>
       <c r="E51">
         <v>0</v>
       </c>
       <c r="F51">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="G51">
-        <v>1.23</v>
+        <v>1.87</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="1">
-        <v>45956.041666667</v>
+        <v>45962.041666667</v>
       </c>
       <c r="B52">
         <v>0</v>
       </c>
       <c r="C52">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="D52">
-        <v>1.44</v>
+        <v>2.21</v>
       </c>
       <c r="E52">
         <v>0</v>
       </c>
       <c r="F52">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="G52">
-        <v>1.23</v>
+        <v>1.87</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="1">
-        <v>45956.083333333</v>
+        <v>45962.083333333</v>
       </c>
       <c r="B53">
         <v>0</v>
       </c>
       <c r="C53">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="D53">
-        <v>1.44</v>
+        <v>2.3</v>
       </c>
       <c r="E53">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="F53">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="G53">
-        <v>1.23</v>
+        <v>2.01</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="1">
-        <v>45956.125</v>
+        <v>45962.125</v>
       </c>
       <c r="B54">
         <v>0</v>
       </c>
       <c r="C54">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="D54">
-        <v>1.52</v>
+        <v>2.3</v>
       </c>
       <c r="E54">
         <v>0</v>
       </c>
       <c r="F54">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="G54">
-        <v>1.12</v>
+        <v>2.01</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="1">
-        <v>45956.166666667</v>
+        <v>45962.166666667</v>
       </c>
       <c r="B55">
         <v>0</v>
       </c>
       <c r="C55">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="D55">
-        <v>1.52</v>
+        <v>2.3</v>
       </c>
       <c r="E55">
         <v>0</v>
       </c>
       <c r="F55">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="G55">
-        <v>1.12</v>
+        <v>2.01</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="1">
-        <v>45956.208333333</v>
+        <v>45962.208333333</v>
       </c>
       <c r="B56">
         <v>0</v>
       </c>
       <c r="C56">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="D56">
-        <v>1.44</v>
+        <v>2.3</v>
       </c>
       <c r="E56">
         <v>0</v>
       </c>
       <c r="F56">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="G56">
-        <v>1.12</v>
+        <v>2.01</v>
       </c>
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="1">
-        <v>45956.25</v>
+        <v>45962.25</v>
       </c>
       <c r="B57">
         <v>0</v>
       </c>
       <c r="C57">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="D57">
-        <v>1.44</v>
+        <v>2.3</v>
       </c>
       <c r="E57">
         <v>0</v>
       </c>
       <c r="F57">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="G57">
-        <v>1.12</v>
+        <v>1.87</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="1">
-        <v>45956.291666667</v>
+        <v>45962.291666667</v>
       </c>
       <c r="B58">
         <v>0</v>
       </c>
       <c r="C58">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="D58">
-        <v>1.44</v>
+        <v>2.3</v>
       </c>
       <c r="E58">
         <v>0</v>
       </c>
       <c r="F58">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="G58">
-        <v>1.23</v>
+        <v>2.01</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="A59" s="1">
-        <v>45956.333333333</v>
+        <v>45962.333333333</v>
       </c>
       <c r="B59">
         <v>0</v>
       </c>
       <c r="C59">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="D59">
-        <v>1.44</v>
+        <v>2.3</v>
       </c>
       <c r="E59">
         <v>0</v>
       </c>
       <c r="F59">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="G59">
-        <v>1.23</v>
+        <v>2.01</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" s="1">
-        <v>45956.375</v>
+        <v>45962.375</v>
       </c>
       <c r="B60">
         <v>0</v>
       </c>
       <c r="C60">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="D60">
-        <v>1.44</v>
+        <v>2.21</v>
       </c>
       <c r="E60">
         <v>0</v>
       </c>
       <c r="F60">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="G60">
-        <v>1.34</v>
+        <v>2.01</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" s="1">
-        <v>45956.416666667</v>
+        <v>45962.416666667</v>
       </c>
       <c r="B61">
         <v>0</v>
       </c>
       <c r="C61">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="D61">
-        <v>1.44</v>
+        <v>2.12</v>
       </c>
       <c r="E61">
         <v>0</v>
       </c>
       <c r="F61">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="G61">
-        <v>1.34</v>
+        <v>2.17</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62" s="1">
-        <v>45956.458333333</v>
+        <v>45962.458333333</v>
       </c>
       <c r="B62">
         <v>0</v>
       </c>
       <c r="C62">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="D62">
-        <v>1.37</v>
+        <v>2.12</v>
       </c>
       <c r="E62">
         <v>0</v>
       </c>
       <c r="F62">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="G62">
-        <v>1.34</v>
+        <v>2.17</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="A63" s="1">
-        <v>45956.5</v>
+        <v>45962.5</v>
       </c>
       <c r="B63">
         <v>0</v>
       </c>
       <c r="C63">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="D63">
-        <v>1.37</v>
+        <v>2.12</v>
       </c>
       <c r="E63">
         <v>0</v>
       </c>
       <c r="F63">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="G63">
-        <v>1.34</v>
+        <v>2.17</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64" s="1">
-        <v>45956.541666667</v>
+        <v>45962.541666667</v>
       </c>
       <c r="B64">
         <v>0</v>
       </c>
       <c r="C64">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="D64">
-        <v>1.44</v>
+        <v>2.12</v>
       </c>
       <c r="E64">
         <v>0</v>
       </c>
       <c r="F64">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="G64">
-        <v>1.34</v>
+        <v>2.17</v>
       </c>
     </row>
     <row r="65" spans="1:7">
       <c r="A65" s="1">
-        <v>45956.583333333</v>
+        <v>45962.583333333</v>
       </c>
       <c r="B65">
         <v>0</v>
       </c>
       <c r="C65">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="D65">
-        <v>1.37</v>
+        <v>2.12</v>
       </c>
       <c r="E65">
         <v>0</v>
       </c>
       <c r="F65">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="G65">
-        <v>1.34</v>
+        <v>2.17</v>
       </c>
     </row>
     <row r="66" spans="1:7">
       <c r="A66" s="1">
-        <v>45956.625</v>
+        <v>45962.625</v>
       </c>
       <c r="B66">
         <v>0</v>
       </c>
       <c r="C66">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="D66">
-        <v>1.44</v>
+        <v>2.12</v>
       </c>
       <c r="E66">
         <v>0</v>
       </c>
       <c r="F66">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="G66">
-        <v>1.34</v>
+        <v>2.17</v>
       </c>
     </row>
     <row r="67" spans="1:7">
       <c r="A67" s="1">
-        <v>45956.666666667</v>
+        <v>45962.666666667</v>
       </c>
       <c r="B67">
         <v>0</v>
       </c>
       <c r="C67">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="D67">
-        <v>1.44</v>
+        <v>2.12</v>
       </c>
       <c r="E67">
         <v>0</v>
       </c>
       <c r="F67">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="G67">
-        <v>1.34</v>
+        <v>2.01</v>
       </c>
     </row>
     <row r="68" spans="1:7">
       <c r="A68" s="1">
-        <v>45956.708333333</v>
+        <v>45962.708333333</v>
       </c>
       <c r="B68">
         <v>0</v>
       </c>
       <c r="C68">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="D68">
-        <v>1.37</v>
+        <v>2.12</v>
       </c>
       <c r="E68">
         <v>0</v>
       </c>
       <c r="F68">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="G68">
-        <v>1.34</v>
+        <v>1.87</v>
       </c>
     </row>
     <row r="69" spans="1:7">
       <c r="A69" s="1">
-        <v>45956.75</v>
+        <v>45962.75</v>
       </c>
       <c r="B69">
         <v>0</v>
       </c>
       <c r="C69">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="D69">
-        <v>1.37</v>
+        <v>2.12</v>
       </c>
       <c r="E69">
         <v>0</v>
       </c>
       <c r="F69">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="G69">
-        <v>1.23</v>
+        <v>1.87</v>
       </c>
     </row>
     <row r="70" spans="1:7">
       <c r="A70" s="1">
-        <v>45956.791666667</v>
+        <v>45962.791666667</v>
       </c>
       <c r="B70">
         <v>0</v>
       </c>
       <c r="C70">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="D70">
-        <v>1.37</v>
+        <v>2.12</v>
       </c>
       <c r="E70">
         <v>0</v>
       </c>
       <c r="F70">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="G70">
-        <v>1.23</v>
+        <v>1.87</v>
       </c>
     </row>
     <row r="71" spans="1:7">
       <c r="A71" s="1">
-        <v>45956.833333333</v>
+        <v>45962.833333333</v>
       </c>
       <c r="B71">
         <v>0</v>
       </c>
       <c r="C71">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="D71">
-        <v>1.37</v>
+        <v>2.12</v>
       </c>
       <c r="E71">
         <v>0</v>
       </c>
       <c r="F71">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="G71">
-        <v>1.23</v>
+        <v>1.87</v>
       </c>
     </row>
     <row r="72" spans="1:7">
       <c r="A72" s="1">
-        <v>45956.875</v>
+        <v>45962.875</v>
       </c>
       <c r="B72">
         <v>0</v>
       </c>
       <c r="C72">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="D72">
-        <v>1.37</v>
+        <v>2.12</v>
       </c>
       <c r="E72">
         <v>0</v>
       </c>
       <c r="F72">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="G72">
-        <v>1.23</v>
+        <v>1.87</v>
       </c>
     </row>
     <row r="73" spans="1:7">
       <c r="A73" s="1">
-        <v>45956.916666667</v>
+        <v>45962.916666667</v>
       </c>
       <c r="B73">
         <v>0</v>
       </c>
       <c r="C73">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="D73">
-        <v>1.37</v>
+        <v>2.03</v>
       </c>
       <c r="E73">
         <v>0</v>
       </c>
       <c r="F73">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="G73">
-        <v>1.23</v>
+        <v>1.87</v>
       </c>
     </row>
     <row r="74" spans="1:7">
       <c r="A74" s="1">
-        <v>45956.958333333</v>
+        <v>45962.958333333</v>
       </c>
       <c r="B74">
         <v>0</v>
       </c>
       <c r="C74">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="D74">
-        <v>1.37</v>
+        <v>2.03</v>
       </c>
       <c r="E74">
         <v>0</v>
       </c>
       <c r="F74">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="G74">
-        <v>1.23</v>
+        <v>1.87</v>
       </c>
     </row>
     <row r="75" spans="1:7">
       <c r="A75" s="1">
-        <v>45957</v>
+        <v>45963</v>
       </c>
       <c r="B75">
         <v>0</v>
       </c>
       <c r="C75">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="D75">
-        <v>1.37</v>
+        <v>1.94</v>
       </c>
       <c r="E75">
         <v>0</v>
       </c>
       <c r="F75">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="G75">
-        <v>1.23</v>
+        <v>1.73</v>
       </c>
     </row>
     <row r="76" spans="1:7">
       <c r="A76" s="1">
-        <v>45957.041666667</v>
+        <v>45963.041666667</v>
       </c>
       <c r="B76">
         <v>0</v>
       </c>
       <c r="C76">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="D76">
-        <v>1.37</v>
+        <v>1.94</v>
       </c>
       <c r="E76">
         <v>0</v>
       </c>
       <c r="F76">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="G76">
-        <v>1.12</v>
+        <v>1.73</v>
       </c>
     </row>
     <row r="77" spans="1:7">
       <c r="A77" s="1">
-        <v>45957.083333333</v>
+        <v>45963.083333333</v>
       </c>
       <c r="B77">
         <v>0</v>
       </c>
       <c r="C77">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="D77">
-        <v>1.44</v>
+        <v>1.94</v>
       </c>
       <c r="E77">
         <v>0</v>
       </c>
       <c r="F77">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="G77">
-        <v>1.12</v>
+        <v>1.73</v>
       </c>
     </row>
     <row r="78" spans="1:7">
       <c r="A78" s="1">
-        <v>45957.125</v>
+        <v>45963.125</v>
       </c>
       <c r="B78">
-        <v>0</v>
+        <v>13.2</v>
       </c>
       <c r="C78">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="D78">
-        <v>1.44</v>
+        <v>2.21</v>
       </c>
       <c r="E78">
         <v>0</v>
       </c>
       <c r="F78">
-        <v>144</v>
+        <v>157</v>
       </c>
       <c r="G78">
-        <v>1.12</v>
+        <v>3.03</v>
       </c>
     </row>
     <row r="79" spans="1:7">
       <c r="A79" s="1">
-        <v>45957.166666667</v>
+        <v>45963.166666667</v>
       </c>
       <c r="B79">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="C79">
-        <v>96</v>
+        <v>186</v>
       </c>
       <c r="D79">
-        <v>1.37</v>
+        <v>15.48</v>
       </c>
       <c r="E79">
         <v>0</v>
       </c>
       <c r="F79">
-        <v>144</v>
+        <v>162</v>
       </c>
       <c r="G79">
-        <v>1.12</v>
+        <v>4.05</v>
       </c>
     </row>
     <row r="80" spans="1:7">
       <c r="A80" s="1">
-        <v>45957.208333333</v>
+        <v>45963.208333333</v>
       </c>
       <c r="B80">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C80">
-        <v>96</v>
+        <v>196</v>
       </c>
       <c r="D80">
-        <v>1.37</v>
+        <v>17.92</v>
       </c>
       <c r="E80">
         <v>0</v>
       </c>
       <c r="F80">
-        <v>144</v>
+        <v>160</v>
       </c>
       <c r="G80">
-        <v>1.12</v>
+        <v>3.62</v>
       </c>
     </row>
     <row r="81" spans="1:7">
       <c r="A81" s="1">
-        <v>45957.25</v>
+        <v>45963.25</v>
       </c>
       <c r="B81">
-        <v>0</v>
+        <v>6.2</v>
       </c>
       <c r="C81">
-        <v>96</v>
+        <v>161</v>
       </c>
       <c r="D81">
-        <v>1.37</v>
+        <v>10.12</v>
       </c>
       <c r="E81">
         <v>0</v>
       </c>
       <c r="F81">
-        <v>144</v>
+        <v>163</v>
       </c>
       <c r="G81">
-        <v>1.12</v>
+        <v>4.28</v>
       </c>
     </row>
     <row r="82" spans="1:7">
       <c r="A82" s="1">
-        <v>45957.291666667</v>
+        <v>45963.291666667</v>
       </c>
       <c r="B82">
         <v>0.4</v>
       </c>
       <c r="C82">
-        <v>97</v>
+        <v>170</v>
       </c>
       <c r="D82">
-        <v>1.44</v>
+        <v>11.93</v>
       </c>
       <c r="E82">
         <v>0</v>
       </c>
       <c r="F82">
-        <v>144</v>
+        <v>161</v>
       </c>
       <c r="G82">
-        <v>1.12</v>
+        <v>3.83</v>
       </c>
     </row>
     <row r="83" spans="1:7">
       <c r="A83" s="1">
-        <v>45957.333333333</v>
+        <v>45963.333333333</v>
       </c>
       <c r="B83">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="C83">
-        <v>96</v>
+        <v>158</v>
       </c>
       <c r="D83">
-        <v>1.37</v>
+        <v>9.55</v>
       </c>
       <c r="E83">
         <v>0</v>
       </c>
       <c r="F83">
-        <v>144</v>
+        <v>160</v>
       </c>
       <c r="G83">
-        <v>1.12</v>
+        <v>3.62</v>
       </c>
     </row>
     <row r="84" spans="1:7">
       <c r="A84" s="1">
-        <v>45957.375</v>
+        <v>45963.375</v>
       </c>
       <c r="B84">
-        <v>0</v>
+        <v>1.6</v>
       </c>
       <c r="C84">
-        <v>97</v>
+        <v>137</v>
       </c>
       <c r="D84">
-        <v>1.44</v>
+        <v>6</v>
       </c>
       <c r="E84">
         <v>0</v>
       </c>
       <c r="F84">
-        <v>144</v>
+        <v>160</v>
       </c>
       <c r="G84">
-        <v>1.12</v>
+        <v>3.62</v>
       </c>
     </row>
     <row r="85" spans="1:7">
       <c r="A85" s="1">
-        <v>45957.416666667</v>
+        <v>45963.416666667</v>
       </c>
       <c r="B85">
-        <v>0.2</v>
+        <v>8.2</v>
       </c>
       <c r="C85">
-        <v>98</v>
+        <v>150</v>
       </c>
       <c r="D85">
-        <v>1.52</v>
+        <v>8.11</v>
       </c>
       <c r="E85">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="F85">
-        <v>144</v>
+        <v>166</v>
       </c>
       <c r="G85">
-        <v>1.12</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="86" spans="1:7">
       <c r="A86" s="1">
-        <v>45957.458333333</v>
+        <v>45963.458333333</v>
       </c>
       <c r="B86">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C86">
-        <v>98</v>
+        <v>192</v>
       </c>
       <c r="D86">
-        <v>1.52</v>
+        <v>16.92</v>
       </c>
       <c r="E86">
         <v>0</v>
       </c>
       <c r="F86">
-        <v>144</v>
+        <v>163</v>
       </c>
       <c r="G86">
-        <v>1.12</v>
+        <v>4.28</v>
       </c>
     </row>
     <row r="87" spans="1:7">
       <c r="A87" s="1">
-        <v>45957.5</v>
+        <v>45963.5</v>
       </c>
       <c r="B87">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C87">
-        <v>97</v>
+        <v>162</v>
       </c>
       <c r="D87">
-        <v>1.44</v>
+        <v>10.31</v>
       </c>
       <c r="E87">
         <v>0</v>
       </c>
       <c r="F87">
-        <v>144</v>
+        <v>163</v>
       </c>
       <c r="G87">
-        <v>1.12</v>
+        <v>4.28</v>
       </c>
     </row>
     <row r="88" spans="1:7">
       <c r="A88" s="1">
-        <v>45957.541666667</v>
+        <v>45963.541666667</v>
       </c>
       <c r="B88">
-        <v>0</v>
+        <v>3.4</v>
       </c>
       <c r="C88">
-        <v>97</v>
+        <v>176</v>
       </c>
       <c r="D88">
-        <v>1.44</v>
+        <v>13.21</v>
       </c>
       <c r="E88">
         <v>0</v>
       </c>
       <c r="F88">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="G88">
-        <v>1.12</v>
+        <v>5.51</v>
       </c>
     </row>
     <row r="89" spans="1:7">
       <c r="A89" s="1">
-        <v>45957.583333333</v>
+        <v>45963.583333333</v>
       </c>
       <c r="B89">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="C89">
-        <v>97</v>
+        <v>193</v>
       </c>
       <c r="D89">
-        <v>1.44</v>
+        <v>17.17</v>
       </c>
       <c r="E89">
         <v>0</v>
       </c>
       <c r="F89">
-        <v>144</v>
+        <v>166</v>
       </c>
       <c r="G89">
-        <v>1.12</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="90" spans="1:7">
       <c r="A90" s="1">
-        <v>45957.625</v>
+        <v>45963.625</v>
       </c>
       <c r="B90">
         <v>0</v>
       </c>
       <c r="C90">
-        <v>97</v>
+        <v>167</v>
       </c>
       <c r="D90">
-        <v>1.44</v>
+        <v>11.31</v>
       </c>
       <c r="E90">
         <v>0</v>
       </c>
       <c r="F90">
-        <v>144</v>
+        <v>166</v>
       </c>
       <c r="G90">
-        <v>1.12</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="91" spans="1:7">
       <c r="A91" s="1">
-        <v>45957.666666667</v>
+        <v>45963.666666667</v>
       </c>
       <c r="B91">
         <v>0</v>
       </c>
       <c r="C91">
-        <v>97</v>
+        <v>149</v>
       </c>
       <c r="D91">
-        <v>1.44</v>
+        <v>7.93</v>
       </c>
       <c r="E91">
         <v>0</v>
       </c>
       <c r="F91">
-        <v>144</v>
+        <v>165</v>
       </c>
       <c r="G91">
-        <v>1.12</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="92" spans="1:7">
       <c r="A92" s="1">
-        <v>45957.708333333</v>
+        <v>45963.708333333</v>
       </c>
       <c r="B92">
         <v>0</v>
       </c>
       <c r="C92">
-        <v>97</v>
+        <v>142</v>
       </c>
       <c r="D92">
-        <v>1.44</v>
+        <v>6.78</v>
       </c>
       <c r="E92">
         <v>0</v>
       </c>
       <c r="F92">
-        <v>144</v>
+        <v>165</v>
       </c>
       <c r="G92">
-        <v>1.12</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="93" spans="1:7">
       <c r="A93" s="1">
-        <v>45957.75</v>
+        <v>45963.75</v>
       </c>
       <c r="B93">
         <v>0</v>
       </c>
       <c r="C93">
-        <v>97</v>
+        <v>139</v>
       </c>
       <c r="D93">
-        <v>1.44</v>
+        <v>6.31</v>
       </c>
       <c r="E93">
         <v>0</v>
       </c>
       <c r="F93">
-        <v>144</v>
+        <v>166</v>
       </c>
       <c r="G93">
-        <v>1.12</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="94" spans="1:7">
       <c r="A94" s="1">
-        <v>45957.791666667</v>
+        <v>45963.791666667</v>
       </c>
       <c r="B94">
         <v>0</v>
       </c>
       <c r="C94">
-        <v>97</v>
+        <v>137</v>
       </c>
       <c r="D94">
-        <v>1.44</v>
+        <v>6</v>
       </c>
       <c r="E94">
         <v>0</v>
       </c>
       <c r="F94">
-        <v>144</v>
+        <v>166</v>
       </c>
       <c r="G94">
-        <v>1.12</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="95" spans="1:7">
       <c r="A95" s="1">
-        <v>45957.833333333</v>
+        <v>45963.833333333</v>
       </c>
       <c r="B95">
         <v>0</v>
       </c>
       <c r="C95">
-        <v>97</v>
+        <v>137</v>
       </c>
       <c r="D95">
-        <v>1.44</v>
+        <v>6</v>
       </c>
       <c r="E95">
         <v>0</v>
       </c>
       <c r="F95">
-        <v>144</v>
+        <v>166</v>
       </c>
       <c r="G95">
-        <v>1.12</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="96" spans="1:7">
       <c r="A96" s="1">
-        <v>45957.875</v>
+        <v>45963.875</v>
       </c>
       <c r="B96">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="C96">
-        <v>98</v>
+        <v>138</v>
       </c>
       <c r="D96">
-        <v>1.52</v>
+        <v>6.15</v>
       </c>
       <c r="E96">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="F96">
-        <v>144</v>
+        <v>167</v>
       </c>
       <c r="G96">
-        <v>1.12</v>
+        <v>5.25</v>
       </c>
     </row>
     <row r="97" spans="1:7">
       <c r="A97" s="1">
-        <v>45957.916666667</v>
+        <v>45963.916666667</v>
       </c>
       <c r="B97">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C97">
-        <v>97</v>
+        <v>137</v>
       </c>
       <c r="D97">
-        <v>1.44</v>
+        <v>6</v>
       </c>
       <c r="E97">
         <v>0</v>
       </c>
       <c r="F97">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="G97">
-        <v>1.12</v>
+        <v>5.51</v>
       </c>
     </row>
     <row r="98" spans="1:7">
       <c r="A98" s="1">
-        <v>45957.958333333</v>
+        <v>45963.958333333</v>
       </c>
       <c r="B98">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="C98">
-        <v>97</v>
+        <v>137</v>
       </c>
       <c r="D98">
-        <v>1.44</v>
+        <v>6</v>
       </c>
       <c r="E98">
         <v>0</v>
       </c>
       <c r="F98">
-        <v>144</v>
+        <v>169</v>
       </c>
       <c r="G98">
-        <v>1.12</v>
+        <v>5.78</v>
       </c>
     </row>
     <row r="99" spans="1:7">
       <c r="A99" s="1">
-        <v>45958</v>
+        <v>45964</v>
       </c>
       <c r="B99">
-        <v>0</v>
+        <v>1.4</v>
       </c>
       <c r="C99">
-        <v>97</v>
+        <v>139</v>
       </c>
       <c r="D99">
-        <v>1.44</v>
+        <v>6.31</v>
       </c>
       <c r="E99">
         <v>0</v>
       </c>
       <c r="F99">
-        <v>145</v>
+        <v>171</v>
       </c>
       <c r="G99">
-        <v>1.23</v>
+        <v>6.33</v>
       </c>
     </row>
     <row r="100" spans="1:7">
       <c r="A100" s="1">
-        <v>45958.041666667</v>
+        <v>45964.041666667</v>
       </c>
       <c r="B100">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C100">
-        <v>97</v>
+        <v>144</v>
       </c>
       <c r="D100">
-        <v>1.44</v>
+        <v>7.1</v>
       </c>
       <c r="E100">
         <v>0</v>
       </c>
       <c r="F100">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="G100">
-        <v>1.23</v>
+        <v>6.62</v>
       </c>
     </row>
     <row r="101" spans="1:7">
       <c r="A101" s="1">
-        <v>45958.083333333</v>
+        <v>45964.083333333</v>
       </c>
       <c r="B101">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C101">
-        <v>98</v>
+        <v>147</v>
       </c>
       <c r="D101">
-        <v>1.52</v>
+        <v>7.59</v>
       </c>
       <c r="E101">
         <v>0</v>
       </c>
       <c r="F101">
-        <v>146</v>
+        <v>174</v>
       </c>
       <c r="G101">
-        <v>1.34</v>
+        <v>7.22</v>
       </c>
     </row>
     <row r="102" spans="1:7">
       <c r="A102" s="1">
-        <v>45958.125</v>
+        <v>45964.125</v>
       </c>
       <c r="B102">
         <v>0.2</v>
       </c>
       <c r="C102">
-        <v>98</v>
+        <v>146</v>
       </c>
       <c r="D102">
-        <v>1.52</v>
+        <v>7.43</v>
       </c>
       <c r="E102">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="F102">
-        <v>146</v>
+        <v>175</v>
       </c>
       <c r="G102">
-        <v>1.34</v>
+        <v>7.53</v>
       </c>
     </row>
     <row r="103" spans="1:7">
       <c r="A103" s="1">
-        <v>45958.166666667</v>
+        <v>45964.166666667</v>
       </c>
       <c r="B103">
         <v>0</v>
       </c>
       <c r="C103">
-        <v>99</v>
+        <v>146</v>
       </c>
       <c r="D103">
-        <v>1.6</v>
+        <v>7.43</v>
       </c>
       <c r="E103">
         <v>0</v>
       </c>
       <c r="F103">
-        <v>146</v>
+        <v>177</v>
       </c>
       <c r="G103">
-        <v>1.34</v>
+        <v>8.18</v>
       </c>
     </row>
     <row r="104" spans="1:7">
       <c r="A104" s="1">
-        <v>45958.208333333</v>
+        <v>45964.208333333</v>
       </c>
       <c r="B104">
         <v>0</v>
       </c>
       <c r="C104">
-        <v>99</v>
+        <v>147</v>
       </c>
       <c r="D104">
-        <v>1.6</v>
+        <v>7.59</v>
       </c>
       <c r="E104">
         <v>0</v>
       </c>
       <c r="F104">
-        <v>146</v>
+        <v>179</v>
       </c>
       <c r="G104">
-        <v>1.34</v>
+        <v>8.85</v>
       </c>
     </row>
     <row r="105" spans="1:7">
       <c r="A105" s="1">
-        <v>45958.25</v>
+        <v>45964.25</v>
       </c>
       <c r="B105">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="C105">
-        <v>99</v>
+        <v>148</v>
       </c>
       <c r="D105">
-        <v>1.6</v>
+        <v>7.76</v>
       </c>
       <c r="E105">
         <v>0</v>
       </c>
       <c r="F105">
-        <v>145</v>
+        <v>180</v>
       </c>
       <c r="G105">
-        <v>1.23</v>
+        <v>9.2</v>
       </c>
     </row>
     <row r="106" spans="1:7">
       <c r="A106" s="1">
-        <v>45958.291666667</v>
+        <v>45964.291666667</v>
       </c>
       <c r="B106">
         <v>0</v>
       </c>
       <c r="C106">
-        <v>99</v>
+        <v>148</v>
       </c>
       <c r="D106">
-        <v>1.6</v>
+        <v>7.76</v>
       </c>
       <c r="E106">
         <v>0</v>
       </c>
       <c r="F106">
-        <v>145</v>
+        <v>184</v>
       </c>
       <c r="G106">
-        <v>1.23</v>
+        <v>10.67</v>
       </c>
     </row>
     <row r="107" spans="1:7">
       <c r="A107" s="1">
-        <v>45958.333333333</v>
+        <v>45964.333333333</v>
       </c>
       <c r="B107">
         <v>0</v>
       </c>
       <c r="C107">
-        <v>99</v>
+        <v>150</v>
       </c>
       <c r="D107">
-        <v>1.6</v>
+        <v>8.11</v>
       </c>
       <c r="E107">
         <v>0</v>
       </c>
       <c r="F107">
-        <v>145</v>
+        <v>182</v>
       </c>
       <c r="G107">
-        <v>1.23</v>
+        <v>9.92</v>
       </c>
     </row>
     <row r="108" spans="1:7">
       <c r="A108" s="1">
-        <v>45958.375</v>
+        <v>45964.375</v>
       </c>
       <c r="B108">
         <v>0</v>
       </c>
       <c r="C108">
-        <v>98</v>
+        <v>150</v>
       </c>
       <c r="D108">
-        <v>1.52</v>
+        <v>8.11</v>
       </c>
       <c r="E108">
         <v>0</v>
       </c>
       <c r="F108">
-        <v>146</v>
+        <v>181</v>
       </c>
       <c r="G108">
-        <v>1.34</v>
+        <v>9.56</v>
       </c>
     </row>
     <row r="109" spans="1:7">
       <c r="A109" s="1">
-        <v>45958.416666667</v>
+        <v>45964.416666667</v>
       </c>
       <c r="B109">
         <v>0</v>
       </c>
       <c r="C109">
-        <v>98</v>
+        <v>149</v>
       </c>
       <c r="D109">
-        <v>1.52</v>
+        <v>7.93</v>
       </c>
       <c r="E109">
         <v>0</v>
       </c>
       <c r="F109">
-        <v>146</v>
+        <v>180</v>
       </c>
       <c r="G109">
-        <v>1.34</v>
+        <v>9.2</v>
       </c>
     </row>
     <row r="110" spans="1:7">
       <c r="A110" s="1">
-        <v>45958.458333333</v>
+        <v>45964.458333333</v>
       </c>
       <c r="B110">
         <v>0</v>
       </c>
       <c r="C110">
-        <v>98</v>
+        <v>148</v>
       </c>
       <c r="D110">
-        <v>1.52</v>
+        <v>7.76</v>
       </c>
       <c r="E110">
         <v>0</v>
       </c>
       <c r="F110">
-        <v>146</v>
+        <v>180</v>
       </c>
       <c r="G110">
-        <v>1.34</v>
+        <v>9.2</v>
       </c>
     </row>
     <row r="111" spans="1:7">
       <c r="A111" s="1">
-        <v>45958.5</v>
+        <v>45964.5</v>
       </c>
       <c r="B111">
         <v>0</v>
       </c>
       <c r="C111">
-        <v>98</v>
+        <v>146</v>
       </c>
       <c r="D111">
-        <v>1.52</v>
+        <v>7.43</v>
       </c>
       <c r="E111">
         <v>0</v>
       </c>
       <c r="F111">
-        <v>146</v>
+        <v>179</v>
       </c>
       <c r="G111">
-        <v>1.34</v>
+        <v>8.85</v>
       </c>
     </row>
     <row r="112" spans="1:7">
       <c r="A112" s="1">
-        <v>45958.541666667</v>
+        <v>45964.541666667</v>
       </c>
       <c r="B112">
         <v>0</v>
       </c>
       <c r="C112">
-        <v>98</v>
+        <v>145</v>
       </c>
       <c r="D112">
-        <v>1.52</v>
+        <v>7.26</v>
       </c>
       <c r="E112">
         <v>0</v>
       </c>
       <c r="F112">
-        <v>146</v>
+        <v>179</v>
       </c>
       <c r="G112">
-        <v>1.34</v>
+        <v>8.85</v>
       </c>
     </row>
     <row r="113" spans="1:7">
       <c r="A113" s="1">
-        <v>45958.583333333</v>
+        <v>45964.583333333</v>
       </c>
       <c r="B113">
         <v>0</v>
       </c>
       <c r="C113">
-        <v>98</v>
+        <v>144</v>
       </c>
       <c r="D113">
-        <v>1.52</v>
+        <v>7.1</v>
       </c>
       <c r="E113">
         <v>0</v>
       </c>
       <c r="F113">
-        <v>146</v>
+        <v>177</v>
       </c>
       <c r="G113">
-        <v>1.34</v>
+        <v>8.18</v>
       </c>
     </row>
     <row r="114" spans="1:7">
       <c r="A114" s="1">
-        <v>45958.625</v>
+        <v>45964.625</v>
       </c>
       <c r="B114">
         <v>0</v>
       </c>
       <c r="C114">
-        <v>98</v>
+        <v>142</v>
       </c>
       <c r="D114">
-        <v>1.52</v>
+        <v>6.78</v>
       </c>
       <c r="E114">
         <v>0</v>
       </c>
       <c r="F114">
-        <v>147</v>
+        <v>177</v>
       </c>
       <c r="G114">
-        <v>1.47</v>
+        <v>8.18</v>
       </c>
     </row>
     <row r="115" spans="1:7">
       <c r="A115" s="1">
-        <v>45958.666666667</v>
+        <v>45964.666666667</v>
       </c>
       <c r="B115">
         <v>0</v>
       </c>
       <c r="C115">
-        <v>98</v>
+        <v>141</v>
       </c>
       <c r="D115">
-        <v>1.52</v>
+        <v>6.62</v>
       </c>
       <c r="E115">
         <v>0</v>
       </c>
       <c r="F115">
-        <v>147</v>
+        <v>176</v>
       </c>
       <c r="G115">
-        <v>1.47</v>
+        <v>7.85</v>
       </c>
     </row>
     <row r="116" spans="1:7">
       <c r="A116" s="1">
-        <v>45958.708333333</v>
+        <v>45964.708333333</v>
       </c>
       <c r="B116">
         <v>0</v>
       </c>
       <c r="C116">
-        <v>98</v>
+        <v>139</v>
       </c>
       <c r="D116">
-        <v>1.52</v>
+        <v>6.31</v>
       </c>
       <c r="E116">
         <v>0</v>
       </c>
       <c r="F116">
-        <v>146</v>
+        <v>175</v>
       </c>
       <c r="G116">
-        <v>1.34</v>
+        <v>7.53</v>
       </c>
     </row>
     <row r="117" spans="1:7">
       <c r="A117" s="1">
-        <v>45958.75</v>
+        <v>45964.75</v>
       </c>
       <c r="B117">
         <v>0</v>
       </c>
       <c r="C117">
-        <v>98</v>
+        <v>138</v>
       </c>
       <c r="D117">
-        <v>1.52</v>
+        <v>6.15</v>
       </c>
       <c r="E117">
         <v>0</v>
       </c>
       <c r="F117">
-        <v>146</v>
+        <v>174</v>
       </c>
       <c r="G117">
-        <v>1.34</v>
+        <v>7.22</v>
       </c>
     </row>
     <row r="118" spans="1:7">
       <c r="A118" s="1">
-        <v>45958.791666667</v>
+        <v>45964.791666667</v>
       </c>
       <c r="B118">
         <v>0</v>
       </c>
       <c r="C118">
-        <v>98</v>
+        <v>137</v>
       </c>
       <c r="D118">
-        <v>1.52</v>
+        <v>6</v>
       </c>
       <c r="E118">
         <v>0</v>
       </c>
       <c r="F118">
-        <v>146</v>
+        <v>172</v>
       </c>
       <c r="G118">
-        <v>1.34</v>
+        <v>6.62</v>
       </c>
     </row>
     <row r="119" spans="1:7">
       <c r="A119" s="1">
-        <v>45958.833333333</v>
+        <v>45964.833333333</v>
       </c>
       <c r="B119">
         <v>0</v>
       </c>
       <c r="C119">
-        <v>99</v>
+        <v>136</v>
       </c>
       <c r="D119">
-        <v>1.6</v>
+        <v>5.85</v>
       </c>
       <c r="E119">
         <v>0</v>
       </c>
       <c r="F119">
-        <v>146</v>
+        <v>172</v>
       </c>
       <c r="G119">
-        <v>1.34</v>
+        <v>6.62</v>
       </c>
     </row>
     <row r="120" spans="1:7">
       <c r="A120" s="1">
-        <v>45958.875</v>
+        <v>45964.875</v>
       </c>
       <c r="B120">
         <v>0</v>
       </c>
       <c r="C120">
-        <v>99</v>
+        <v>134</v>
       </c>
       <c r="D120">
-        <v>1.6</v>
+        <v>5.56</v>
       </c>
       <c r="E120">
         <v>0</v>
       </c>
       <c r="F120">
-        <v>146</v>
+        <v>171</v>
       </c>
       <c r="G120">
-        <v>1.34</v>
+        <v>6.33</v>
       </c>
     </row>
     <row r="121" spans="1:7">
       <c r="A121" s="1">
-        <v>45958.916666667</v>
+        <v>45964.916666667</v>
       </c>
       <c r="B121">
         <v>0</v>
       </c>
       <c r="C121">
-        <v>99</v>
+        <v>133</v>
       </c>
       <c r="D121">
-        <v>1.6</v>
+        <v>5.41</v>
       </c>
       <c r="E121">
         <v>0</v>
       </c>
       <c r="F121">
-        <v>146</v>
+        <v>170</v>
       </c>
       <c r="G121">
-        <v>1.34</v>
+        <v>6.05</v>
       </c>
     </row>
     <row r="122" spans="1:7">
       <c r="A122" s="1">
-        <v>45958.958333333</v>
+        <v>45964.958333333</v>
       </c>
       <c r="B122">
         <v>0</v>
       </c>
       <c r="C122">
-        <v>99</v>
+        <v>132</v>
       </c>
       <c r="D122">
-        <v>1.6</v>
+        <v>5.27</v>
       </c>
       <c r="E122">
         <v>0</v>
       </c>
       <c r="F122">
-        <v>146</v>
+        <v>169</v>
       </c>
       <c r="G122">
-        <v>1.34</v>
+        <v>5.78</v>
       </c>
     </row>
     <row r="123" spans="1:7">
       <c r="A123" s="1">
-        <v>45959</v>
+        <v>45965</v>
       </c>
       <c r="B123">
         <v>0</v>
       </c>
       <c r="C123">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="D123">
-        <v>1.52</v>
+        <v>4.99</v>
       </c>
       <c r="E123">
         <v>0</v>
       </c>
       <c r="F123">
-        <v>146</v>
+        <v>169</v>
       </c>
       <c r="G123">
-        <v>1.34</v>
+        <v>5.78</v>
       </c>
     </row>
     <row r="124" spans="1:7">
       <c r="A124" s="1">
-        <v>45959.041666667</v>
+        <v>45965.041666667</v>
       </c>
       <c r="B124">
         <v>0</v>
       </c>
       <c r="C124">
-        <v>98</v>
+        <v>129</v>
       </c>
       <c r="D124">
-        <v>1.52</v>
+        <v>4.86</v>
       </c>
       <c r="E124">
         <v>0</v>
       </c>
       <c r="F124">
-        <v>146</v>
+        <v>168</v>
       </c>
       <c r="G124">
-        <v>1.34</v>
+        <v>5.51</v>
       </c>
     </row>
     <row r="125" spans="1:7">
       <c r="A125" s="1">
-        <v>45959.083333333</v>
+        <v>45965.083333333</v>
       </c>
       <c r="B125">
         <v>0</v>
       </c>
       <c r="C125">
-        <v>98</v>
+        <v>129</v>
       </c>
       <c r="D125">
-        <v>1.52</v>
+        <v>4.86</v>
       </c>
       <c r="E125">
         <v>0</v>
       </c>
       <c r="F125">
-        <v>146</v>
+        <v>168</v>
       </c>
       <c r="G125">
-        <v>1.34</v>
+        <v>5.51</v>
       </c>
     </row>
     <row r="126" spans="1:7">
       <c r="A126" s="1">
-        <v>45959.125</v>
+        <v>45965.125</v>
       </c>
       <c r="B126">
-        <v>11.4</v>
+        <v>0</v>
       </c>
       <c r="C126">
-        <v>101</v>
+        <v>129</v>
       </c>
       <c r="D126">
-        <v>1.76</v>
+        <v>4.86</v>
       </c>
       <c r="E126">
         <v>0</v>
       </c>
       <c r="F126">
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="G126">
-        <v>1.73</v>
+        <v>5.25</v>
       </c>
     </row>
     <row r="127" spans="1:7">
       <c r="A127" s="1">
-        <v>45959.166666667</v>
+        <v>45965.166666667</v>
       </c>
       <c r="B127">
-        <v>7.4</v>
+        <v>0</v>
       </c>
       <c r="C127">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D127">
-        <v>4.86</v>
+        <v>4.59</v>
       </c>
       <c r="E127">
         <v>0</v>
       </c>
       <c r="F127">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="G127">
-        <v>3.22</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="128" spans="1:7">
       <c r="A128" s="1">
-        <v>45959.208333333</v>
+        <v>45965.208333333</v>
       </c>
       <c r="B128">
         <v>0</v>
       </c>
       <c r="C128">
-        <v>183</v>
+        <v>126</v>
       </c>
       <c r="D128">
-        <v>14.78</v>
+        <v>4.46</v>
       </c>
       <c r="E128">
         <v>0</v>
       </c>
       <c r="F128">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="G128">
-        <v>3.03</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="129" spans="1:7">
       <c r="A129" s="1">
-        <v>45959.25</v>
+        <v>45965.25</v>
       </c>
       <c r="B129">
         <v>0</v>
       </c>
       <c r="C129">
-        <v>147</v>
+        <v>125</v>
       </c>
       <c r="D129">
-        <v>7.59</v>
+        <v>4.33</v>
       </c>
       <c r="E129">
         <v>0</v>
       </c>
       <c r="F129">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="G129">
-        <v>2.49</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="130" spans="1:7">
       <c r="A130" s="1">
-        <v>45959.291666667</v>
+        <v>45965.291666667</v>
       </c>
       <c r="B130">
         <v>0</v>
       </c>
       <c r="C130">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D130">
-        <v>4.33</v>
+        <v>4.2</v>
       </c>
       <c r="E130">
         <v>0</v>
       </c>
       <c r="F130">
-        <v>152</v>
+        <v>165</v>
       </c>
       <c r="G130">
-        <v>2.17</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="131" spans="1:7">
       <c r="A131" s="1">
-        <v>45959.333333333</v>
+        <v>45965.333333333</v>
       </c>
       <c r="B131">
         <v>0</v>
       </c>
       <c r="C131">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D131">
-        <v>3.47</v>
+        <v>4.07</v>
       </c>
       <c r="E131">
         <v>0</v>
       </c>
       <c r="F131">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="G131">
-        <v>2.01</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="132" spans="1:7">
       <c r="A132" s="1">
-        <v>45959.375</v>
+        <v>45965.375</v>
       </c>
       <c r="B132">
         <v>0</v>
       </c>
       <c r="C132">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="D132">
-        <v>2.91</v>
+        <v>3.95</v>
       </c>
       <c r="E132">
         <v>0</v>
       </c>
       <c r="F132">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="G132">
-        <v>1.87</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="133" spans="1:7">
       <c r="A133" s="1">
-        <v>45959.416666667</v>
+        <v>45965.416666667</v>
       </c>
       <c r="B133">
         <v>0</v>
       </c>
       <c r="C133">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="D133">
-        <v>2.5</v>
+        <v>3.95</v>
       </c>
       <c r="E133">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="F133">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="G133">
-        <v>1.87</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="134" spans="1:7">
       <c r="A134" s="1">
-        <v>45959.458333333</v>
+        <v>45965.458333333</v>
       </c>
       <c r="B134">
         <v>0</v>
       </c>
       <c r="C134">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="D134">
-        <v>2.3</v>
+        <v>3.82</v>
       </c>
       <c r="E134">
         <v>0</v>
       </c>
       <c r="F134">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="G134">
-        <v>1.73</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="135" spans="1:7">
       <c r="A135" s="1">
-        <v>45959.5</v>
+        <v>45965.5</v>
       </c>
       <c r="B135">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C135">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="D135">
-        <v>2.21</v>
+        <v>3.82</v>
       </c>
       <c r="E135">
         <v>0</v>
       </c>
       <c r="F135">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="G135">
-        <v>1.73</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="136" spans="1:7">
       <c r="A136" s="1">
-        <v>45959.541666667</v>
+        <v>45965.541666667</v>
       </c>
       <c r="B136">
-        <v>1.4</v>
+        <v>0</v>
       </c>
       <c r="C136">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="D136">
-        <v>2.6</v>
+        <v>3.82</v>
       </c>
       <c r="E136">
         <v>0</v>
       </c>
       <c r="F136">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="G136">
-        <v>1.87</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="137" spans="1:7">
       <c r="A137" s="1">
-        <v>45959.583333333</v>
+        <v>45965.583333333</v>
       </c>
       <c r="B137">
         <v>0</v>
       </c>
       <c r="C137">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="D137">
-        <v>3.35</v>
+        <v>3.82</v>
       </c>
       <c r="E137">
         <v>0</v>
       </c>
       <c r="F137">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="G137">
-        <v>1.87</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="138" spans="1:7">
       <c r="A138" s="1">
-        <v>45959.625</v>
+        <v>45965.625</v>
       </c>
       <c r="B138">
         <v>0</v>
       </c>
       <c r="C138">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="D138">
-        <v>2.91</v>
+        <v>3.82</v>
       </c>
       <c r="E138">
         <v>0</v>
       </c>
       <c r="F138">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="G138">
-        <v>1.87</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="139" spans="1:7">
       <c r="A139" s="1">
-        <v>45959.666666667</v>
+        <v>45965.666666667</v>
       </c>
       <c r="B139">
         <v>0</v>
       </c>
       <c r="C139">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="D139">
-        <v>2.4</v>
+        <v>3.82</v>
       </c>
       <c r="E139">
         <v>0</v>
       </c>
       <c r="F139">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="G139">
-        <v>1.87</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="140" spans="1:7">
       <c r="A140" s="1">
-        <v>45959.708333333</v>
+        <v>45965.708333333</v>
       </c>
       <c r="B140">
         <v>0</v>
       </c>
       <c r="C140">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="D140">
-        <v>2.21</v>
+        <v>3.95</v>
       </c>
       <c r="E140">
         <v>0</v>
       </c>
       <c r="F140">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="G140">
-        <v>1.87</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="141" spans="1:7">
       <c r="A141" s="1">
-        <v>45959.75</v>
+        <v>45965.75</v>
       </c>
       <c r="B141">
         <v>0</v>
       </c>
       <c r="C141">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="D141">
-        <v>2.21</v>
+        <v>3.95</v>
       </c>
       <c r="E141">
         <v>0</v>
       </c>
       <c r="F141">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="G141">
-        <v>1.87</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="142" spans="1:7">
       <c r="A142" s="1">
-        <v>45959.791666667</v>
+        <v>45965.791666667</v>
       </c>
       <c r="B142">
         <v>0</v>
       </c>
       <c r="C142">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="D142">
-        <v>2.21</v>
+        <v>3.95</v>
       </c>
       <c r="E142">
         <v>0</v>
       </c>
       <c r="F142">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="G142">
-        <v>1.87</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="143" spans="1:7">
       <c r="A143" s="1">
-        <v>45959.833333333</v>
+        <v>45965.833333333</v>
       </c>
       <c r="B143">
         <v>0</v>
       </c>
       <c r="C143">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="D143">
-        <v>2.21</v>
+        <v>3.95</v>
       </c>
       <c r="E143">
         <v>0</v>
       </c>
       <c r="F143">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="G143">
-        <v>1.87</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="144" spans="1:7">
       <c r="A144" s="1">
-        <v>45959.875</v>
+        <v>45965.875</v>
       </c>
       <c r="B144">
         <v>0</v>
       </c>
       <c r="C144">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="D144">
-        <v>2.21</v>
+        <v>3.95</v>
       </c>
       <c r="E144">
         <v>0</v>
       </c>
       <c r="F144">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="G144">
-        <v>1.87</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="145" spans="1:7">
       <c r="A145" s="1">
-        <v>45959.916666667</v>
+        <v>45965.916666667</v>
       </c>
       <c r="B145">
         <v>0</v>
       </c>
       <c r="C145">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="D145">
-        <v>2.12</v>
+        <v>3.95</v>
       </c>
       <c r="E145">
         <v>0</v>
       </c>
       <c r="F145">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="G145">
-        <v>1.87</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="146" spans="1:7">
       <c r="A146" s="1">
-        <v>45959.958333333</v>
+        <v>45965.958333333</v>
       </c>
       <c r="B146">
         <v>0</v>
       </c>
       <c r="C146">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="D146">
-        <v>2.12</v>
+        <v>3.82</v>
       </c>
       <c r="E146">
         <v>0</v>
       </c>
       <c r="F146">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="G146">
-        <v>1.87</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="147" spans="1:7">
       <c r="A147" s="1">
-        <v>45960</v>
+        <v>45966</v>
       </c>
       <c r="B147">
         <v>0</v>
       </c>
       <c r="C147">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="D147">
-        <v>2.12</v>
+        <v>3.95</v>
       </c>
       <c r="E147">
         <v>0</v>
       </c>
       <c r="F147">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="G147">
-        <v>1.87</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="148" spans="1:7">
       <c r="A148" s="1">
-        <v>45960.041666667</v>
+        <v>45966.041666667</v>
       </c>
       <c r="B148">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="C148">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="D148">
-        <v>2.12</v>
+        <v>3.95</v>
       </c>
       <c r="E148">
         <v>0</v>
       </c>
       <c r="F148">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="G148">
-        <v>1.87</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="149" spans="1:7">
       <c r="A149" s="1">
-        <v>45960.083333333</v>
+        <v>45966.083333333</v>
       </c>
       <c r="B149">
         <v>0</v>
       </c>
       <c r="C149">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="D149">
-        <v>2.12</v>
+        <v>4.07</v>
       </c>
       <c r="E149">
         <v>0</v>
       </c>
       <c r="F149">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="G149">
-        <v>1.87</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="150" spans="1:7">
       <c r="A150" s="1">
-        <v>45960.125</v>
+        <v>45966.125</v>
       </c>
       <c r="B150">
         <v>0</v>
       </c>
       <c r="C150">
-        <v>105</v>
+        <v>124</v>
       </c>
       <c r="D150">
-        <v>2.12</v>
+        <v>4.2</v>
       </c>
       <c r="E150">
         <v>0</v>
       </c>
       <c r="F150">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="G150">
-        <v>1.73</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="151" spans="1:7">
       <c r="A151" s="1">
-        <v>45960.166666667</v>
+        <v>45966.166666667</v>
       </c>
       <c r="B151">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C151">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="D151">
-        <v>2.12</v>
+        <v>4.07</v>
       </c>
       <c r="E151">
         <v>0</v>
       </c>
       <c r="F151">
-        <v>149</v>
+        <v>164</v>
       </c>
       <c r="G151">
-        <v>1.73</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="152" spans="1:7">
       <c r="A152" s="1">
-        <v>45960.208333333</v>
+        <v>45966.208333333</v>
       </c>
       <c r="B152">
         <v>0</v>
       </c>
       <c r="C152">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="D152">
-        <v>2.12</v>
+        <v>3.95</v>
       </c>
       <c r="E152">
         <v>0</v>
       </c>
       <c r="F152">
-        <v>149</v>
+        <v>164</v>
       </c>
       <c r="G152">
-        <v>1.73</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="153" spans="1:7">
       <c r="A153" s="1">
-        <v>45960.25</v>
+        <v>45966.25</v>
       </c>
       <c r="B153">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="C153">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="D153">
-        <v>2.12</v>
+        <v>3.95</v>
       </c>
       <c r="E153">
         <v>0</v>
       </c>
       <c r="F153">
-        <v>150</v>
+        <v>164</v>
       </c>
       <c r="G153">
-        <v>1.87</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="154" spans="1:7">
       <c r="A154" s="1">
-        <v>45960.291666667</v>
+        <v>45966.291666667</v>
       </c>
       <c r="B154">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C154">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="D154">
-        <v>2.21</v>
+        <v>3.82</v>
       </c>
       <c r="E154">
         <v>0</v>
       </c>
       <c r="F154">
-        <v>149</v>
+        <v>164</v>
       </c>
       <c r="G154">
-        <v>1.73</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="155" spans="1:7">
       <c r="A155" s="1">
-        <v>45960.333333333</v>
+        <v>45966.333333333</v>
       </c>
       <c r="B155">
         <v>0</v>
       </c>
       <c r="C155">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="D155">
-        <v>2.4</v>
+        <v>3.82</v>
       </c>
       <c r="E155">
         <v>0</v>
       </c>
       <c r="F155">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="G155">
-        <v>1.73</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="156" spans="1:7">
       <c r="A156" s="1">
-        <v>45960.375</v>
+        <v>45966.375</v>
       </c>
       <c r="B156">
         <v>0</v>
       </c>
       <c r="C156">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="D156">
-        <v>2.3</v>
+        <v>3.82</v>
       </c>
       <c r="E156">
         <v>0</v>
       </c>
       <c r="F156">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="G156">
-        <v>1.87</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="157" spans="1:7">
       <c r="A157" s="1">
-        <v>45960.416666667</v>
+        <v>45966.416666667</v>
       </c>
       <c r="B157">
         <v>0</v>
       </c>
       <c r="C157">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="D157">
-        <v>2.12</v>
+        <v>3.82</v>
       </c>
       <c r="E157">
         <v>0</v>
       </c>
       <c r="F157">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="G157">
-        <v>1.87</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="158" spans="1:7">
       <c r="A158" s="1">
-        <v>45960.458333333</v>
+        <v>45966.458333333</v>
       </c>
       <c r="B158">
         <v>0</v>
       </c>
       <c r="C158">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="D158">
-        <v>2.12</v>
+        <v>3.82</v>
       </c>
       <c r="E158">
         <v>0</v>
       </c>
       <c r="F158">
-        <v>150</v>
+        <v>164</v>
       </c>
       <c r="G158">
-        <v>1.87</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="159" spans="1:7">
       <c r="A159" s="1">
-        <v>45960.5</v>
+        <v>45966.5</v>
       </c>
       <c r="B159">
         <v>0</v>
       </c>
       <c r="C159">
-        <v>104</v>
+        <v>121</v>
       </c>
       <c r="D159">
-        <v>2.03</v>
+        <v>3.82</v>
       </c>
       <c r="E159">
         <v>0</v>
       </c>
       <c r="F159">
-        <v>150</v>
+        <v>164</v>
       </c>
       <c r="G159">
-        <v>1.87</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="160" spans="1:7">
       <c r="A160" s="1">
-        <v>45960.541666667</v>
+        <v>45966.541666667</v>
       </c>
       <c r="B160">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C160">
-        <v>104</v>
+        <v>121</v>
       </c>
       <c r="D160">
-        <v>2.03</v>
+        <v>3.82</v>
       </c>
       <c r="E160">
         <v>0</v>
       </c>
       <c r="F160">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="G160">
-        <v>1.87</v>
+        <v>4.28</v>
       </c>
     </row>
     <row r="161" spans="1:7">
       <c r="A161" s="1">
-        <v>45960.583333333</v>
+        <v>45966.583333333</v>
       </c>
       <c r="B161">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="C161">
-        <v>104</v>
+        <v>121</v>
       </c>
       <c r="D161">
-        <v>2.03</v>
+        <v>3.82</v>
       </c>
       <c r="E161">
         <v>0</v>
       </c>
       <c r="F161">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="G161">
-        <v>1.87</v>
+        <v>4.28</v>
       </c>
     </row>
     <row r="162" spans="1:7">
       <c r="A162" s="1">
-        <v>45960.625</v>
+        <v>45966.625</v>
       </c>
       <c r="B162">
         <v>0</v>
       </c>
       <c r="C162">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="D162">
-        <v>2.03</v>
+        <v>4.07</v>
       </c>
       <c r="E162">
         <v>0</v>
       </c>
       <c r="F162">
-        <v>149</v>
+        <v>163</v>
       </c>
       <c r="G162">
-        <v>1.73</v>
+        <v>4.28</v>
       </c>
     </row>
     <row r="163" spans="1:7">
       <c r="A163" s="1">
-        <v>45960.666666667</v>
+        <v>45966.666666667</v>
       </c>
       <c r="B163">
         <v>0</v>
       </c>
       <c r="C163">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="D163">
-        <v>2.03</v>
+        <v>3.95</v>
       </c>
       <c r="E163">
         <v>0</v>
       </c>
       <c r="F163">
-        <v>149</v>
+        <v>163</v>
       </c>
       <c r="G163">
-        <v>1.73</v>
+        <v>4.28</v>
       </c>
     </row>
     <row r="164" spans="1:7">
       <c r="A164" s="1">
-        <v>45960.708333333</v>
+        <v>45966.708333333</v>
       </c>
       <c r="B164">
         <v>0</v>
       </c>
       <c r="C164">
-        <v>104</v>
+        <v>121</v>
       </c>
       <c r="D164">
-        <v>2.03</v>
+        <v>3.82</v>
       </c>
       <c r="E164">
         <v>0</v>
       </c>
       <c r="F164">
-        <v>149</v>
+        <v>163</v>
       </c>
       <c r="G164">
-        <v>1.73</v>
+        <v>4.28</v>
       </c>
     </row>
     <row r="165" spans="1:7">
       <c r="A165" s="1">
-        <v>45960.75</v>
+        <v>45966.75</v>
       </c>
       <c r="B165">
         <v>0</v>
       </c>
       <c r="C165">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="D165">
-        <v>2.03</v>
+        <v>3.7</v>
       </c>
       <c r="E165">
         <v>0</v>
       </c>
       <c r="F165">
-        <v>149</v>
+        <v>162</v>
       </c>
       <c r="G165">
-        <v>1.73</v>
+        <v>4.05</v>
       </c>
     </row>
     <row r="166" spans="1:7">
       <c r="A166" s="1">
-        <v>45960.791666667</v>
+        <v>45966.791666667</v>
       </c>
       <c r="B166">
         <v>0</v>
       </c>
       <c r="C166">
-        <v>104</v>
+        <v>119</v>
       </c>
       <c r="D166">
-        <v>2.03</v>
+        <v>3.59</v>
       </c>
       <c r="E166">
         <v>0</v>
       </c>
       <c r="F166">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="G166">
-        <v>1.73</v>
+        <v>3.83</v>
       </c>
     </row>
     <row r="167" spans="1:7">
       <c r="A167" s="1">
-        <v>45960.833333333</v>
+        <v>45966.833333333</v>
       </c>
       <c r="B167">
         <v>0</v>
       </c>
       <c r="C167">
-        <v>104</v>
+        <v>119</v>
       </c>
       <c r="D167">
-        <v>2.03</v>
+        <v>3.59</v>
       </c>
       <c r="E167">
         <v>0</v>
       </c>
       <c r="F167">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="G167">
-        <v>1.73</v>
+        <v>3.83</v>
       </c>
     </row>
     <row r="168" spans="1:7">
       <c r="A168" s="1">
-        <v>45960.875</v>
+        <v>45966.875</v>
       </c>
       <c r="B168">
         <v>0</v>
       </c>
       <c r="C168">
-        <v>104</v>
+        <v>119</v>
       </c>
       <c r="D168">
-        <v>2.03</v>
+        <v>3.59</v>
       </c>
       <c r="E168">
         <v>0</v>
       </c>
       <c r="F168">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="G168">
-        <v>1.73</v>
+        <v>3.83</v>
       </c>
     </row>
     <row r="169" spans="1:7">
       <c r="A169" s="1">
-        <v>45960.916666667</v>
+        <v>45966.916666667</v>
       </c>
       <c r="B169">
         <v>0</v>
       </c>
       <c r="C169">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="D169">
-        <v>2.03</v>
+        <v>3.47</v>
       </c>
       <c r="E169">
         <v>0</v>
       </c>
       <c r="F169">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="G169">
-        <v>1.73</v>
+        <v>3.62</v>
       </c>
     </row>
     <row r="170" spans="1:7">
       <c r="A170" s="2">
-        <v>45960.958333333</v>
+        <v>45966.958333333</v>
       </c>
       <c r="B170" s="3">
         <v>0</v>
       </c>
       <c r="C170" s="3">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="D170" s="3">
-        <v>1.94</v>
+        <v>3.47</v>
       </c>
       <c r="E170" s="3">
         <v>0</v>
       </c>
       <c r="F170" s="3">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="G170" s="3">
-        <v>1.59</v>
+        <v>3.62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>